<commit_message>
Stricter constraints on max DMI intake
</commit_message>
<xml_diff>
--- a/workbooks/base.xlsx
+++ b/workbooks/base.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="107">
   <si>
     <t>f_crop</t>
   </si>
@@ -288,6 +288,9 @@
     <t>f_breed</t>
   </si>
   <si>
+    <t>f_animal</t>
+  </si>
+  <si>
     <t>cows</t>
   </si>
   <si>
@@ -324,7 +327,28 @@
     <t>beef</t>
   </si>
   <si>
-    <t>Fix grazing</t>
+    <t>Fixed grazing</t>
+  </si>
+  <si>
+    <t>Refine max DMI intakes</t>
+  </si>
+  <si>
+    <t>calves, bull</t>
+  </si>
+  <si>
+    <t>calves, for slaughter</t>
+  </si>
+  <si>
+    <t>calves, heifer</t>
+  </si>
+  <si>
+    <t>calves, steer</t>
+  </si>
+  <si>
+    <t>max_DMI</t>
+  </si>
+  <si>
+    <t>abs</t>
   </si>
 </sst>
 </file>
@@ -407,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -420,6 +444,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -4636,909 +4662,1261 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="1" t="s">
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="1" t="s">
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="1" t="s">
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="1" t="s">
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
-      <c r="I32" s="1" t="s">
+      <c r="G32" s="1"/>
+      <c r="J32" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="1" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="1" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="1" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="1" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="1" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I38" s="1" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="1" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41">
-        <v>0.7</v>
-      </c>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>0.75</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>88</v>
+      <c r="C42" t="s">
+        <v>87</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42">
+        <v>89</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="11">
         <v>0.5</v>
       </c>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
-      <c r="B43" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44">
-        <v>0.6</v>
-      </c>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="E47"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
-      <c r="B48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>31</v>
       </c>
-      <c r="E48" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="12">
         <v>6.6079520088655128</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
-      <c r="B49" t="s">
-        <v>94</v>
-      </c>
       <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" t="s">
         <v>38</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>31</v>
       </c>
-      <c r="E49" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="11">
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="13">
         <v>50.052481882315824</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
-      <c r="B50" t="s">
-        <v>90</v>
-      </c>
       <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
         <v>38</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>31</v>
       </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="11">
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
-      <c r="B51" t="s">
-        <v>95</v>
-      </c>
       <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
         <v>38</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>31</v>
       </c>
-      <c r="E51" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="11">
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="13">
         <v>37.985802806201164</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
-      <c r="B52" t="s">
-        <v>96</v>
-      </c>
       <c r="C52" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" t="s">
         <v>38</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>31</v>
       </c>
-      <c r="E52" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="11">
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="13">
         <v>38.614788214420173</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="13">
+        <v>58.050981669759572</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="13">
+        <v>50.052481882315824</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" t="s">
         <v>91</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D56" t="s">
         <v>38</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E56" t="s">
         <v>31</v>
       </c>
-      <c r="E53" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="11">
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="13">
+        <v>30.425854259446911</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="13">
+        <v>30.282083494235561</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="9"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G61" s="10">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62" s="10">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G63" s="10">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G64" s="10">
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" s="10">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="10">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G67" s="10">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" s="10">
+        <v>19.190000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69" s="10">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B54" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" t="s">
-        <v>38</v>
-      </c>
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="11">
-        <v>58.050981669759572</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="E70" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G70" s="10">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G71" s="10">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G72" s="10">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>98</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G73" s="10">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G74" s="10">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G75" s="10">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G76" s="10">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G77" s="10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>98</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G78" s="10">
+        <v>10.77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G79" s="10">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E55" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="11">
-        <v>50.052481882315824</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" t="s">
-        <v>8</v>
-      </c>
-      <c r="F56" s="11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="11">
-        <v>30.425854259446911</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" s="11">
-        <v>30.282083494235561</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" t="s">
-        <v>31</v>
-      </c>
-      <c r="E59" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" s="11">
-        <v>0</v>
+      <c r="E80" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G80" s="10">
+        <v>7.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>